<commit_message>
Done with product cancellation
Done with product cancellation
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\way2automation\PycharmProjects\AppiumPageObjectModel\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\appium-python-pytest\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866D82B9-715C-453D-B1F1-0A1A6D10D98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="730" yWindow="730" windowWidth="17280" windowHeight="8960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SearchTest" sheetId="1" r:id="rId1"/>
     <sheet name="VillaTest" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductSearch" sheetId="3" r:id="rId3"/>
+    <sheet name="CardDetails" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>city</t>
   </si>
@@ -40,11 +41,41 @@
   <si>
     <t>Savoy Suites Hotel Apartment</t>
   </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>OSSOBERRY Micro USB, USB Type C, Lightning OTG Adapter</t>
+  </si>
+  <si>
+    <t>OSSOBERRY Micro USB, USB Type C, Lightning OTG Adapter (Pack of 1)</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Card No</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>02/30</t>
+  </si>
+  <si>
+    <t>4315813955699002</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,26 +421,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -419,16 +451,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B07524-A26A-420B-871C-7D4A984E16B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -444,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -455,4 +490,85 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="59.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>